<commit_message>
Full Project including advanced topic
</commit_message>
<xml_diff>
--- a/src/main/java/data.xlsx
+++ b/src/main/java/data.xlsx
@@ -4,28 +4,38 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14175" windowHeight="6120"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
-  <si>
-    <t>admin</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
   <si>
     <t>admin123</t>
   </si>
   <si>
     <t>tutorial</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>This is a test</t>
+  </si>
+  <si>
+    <t>Cassidy Hope</t>
+  </si>
+  <si>
+    <t>US - FMLA</t>
   </si>
 </sst>
 </file>
@@ -369,26 +379,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" activeCellId="1" sqref="B1 D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -398,26 +408,50 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>2020</v>
+      </c>
+      <c r="E1">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1">
+        <v>2020</v>
+      </c>
+      <c r="H1">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>